<commit_message>
Resultaten_statistiek: correction formula for visualisation significant p-values
</commit_message>
<xml_diff>
--- a/data/Resultaten_Statistiek.xlsx
+++ b/data/Resultaten_Statistiek.xlsx
@@ -215,7 +215,45 @@
     <cellStyle name="Berekening" xfId="1" builtinId="22"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -558,7 +596,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,22 +1121,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B30">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>IF(B2 &lt;0.01, IF(C2&gt;0,1,0),0) &gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>IF(B2 &lt;0.01, IF(C2&lt;0,1,0),0) &gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>IF(B3 &lt;0.05, IF(C3&gt;0,1,0),0) &gt;0</formula>
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>IF(B2 &lt;0.05, IF(C2&gt;0,1,0),0) &gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>IF(B3 &lt;0.05, IF(C3&lt;0,1,0),0) &gt;0</formula>
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>IF(B2 &lt;0.05, IF(C2&lt;0,1,0),0) &gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>